<commit_message>
fixed case problem in dlc sheet
</commit_message>
<xml_diff>
--- a/wetb/dlc/tests/test_files/DLC_test.xlsx
+++ b/wetb/dlc/tests/test_files/DLC_test.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="23610" windowHeight="7695" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="23610" windowHeight="7695" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DLC" sheetId="1" r:id="rId1"/>
     <sheet name="Sensors" sheetId="3" r:id="rId2"/>
     <sheet name="Variables" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
@@ -228,9 +228,6 @@
     <t>res_folder</t>
   </si>
   <si>
-    <t>DLC%s_IEC61400-1ed3</t>
-  </si>
-  <si>
     <t>Folder name pattern for result files, e.g. DLC%s_IEC61400-1ed3, where '%s' will be replace with dlc group id</t>
   </si>
   <si>
@@ -337,16 +334,19 @@
   </si>
   <si>
     <t>MinDistance</t>
+  </si>
+  <si>
+    <t>dlc%s_iec61400-1ed3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0E+00"/>
+    <numFmt numFmtId="172" formatCode="0E+00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -394,7 +394,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor indexed="55"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,19 +417,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -462,6 +449,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -484,7 +484,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -497,27 +497,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -561,11 +561,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -644,7 +639,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -679,7 +673,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -855,15 +848,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD6"/>
+      <selection activeCell="A3" sqref="A3:IV6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
@@ -876,7 +869,7 @@
     <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="32" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="32" customFormat="1" ht="13.5" thickBot="1">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -884,19 +877,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>3</v>
@@ -911,68 +904,68 @@
         <v>6</v>
       </c>
       <c r="L1" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>94</v>
       </c>
       <c r="P1" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="33" customFormat="1" ht="48.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="33" customFormat="1" ht="48.75" thickBot="1">
       <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F2" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="H2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>45</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" s="34" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:16" s="34" customFormat="1" ht="13.5" thickBot="1">
       <c r="A3" s="26" t="s">
         <v>13</v>
       </c>
@@ -1022,7 +1015,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="34" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="34" customFormat="1" ht="13.5" thickBot="1">
       <c r="A4" s="26" t="s">
         <v>15</v>
       </c>
@@ -1066,7 +1059,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="34" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="34" customFormat="1" ht="13.5" thickBot="1">
       <c r="A5" s="26" t="s">
         <v>57</v>
       </c>
@@ -1108,7 +1101,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="34" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="34" customFormat="1" ht="13.5" thickBot="1">
       <c r="A6" s="26" t="s">
         <v>18</v>
       </c>
@@ -1143,10 +1136,10 @@
         <v>12</v>
       </c>
       <c r="L6" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" s="26" t="s">
         <v>72</v>
-      </c>
-      <c r="M6" s="26" t="s">
-        <v>73</v>
       </c>
       <c r="N6" s="26">
         <v>100</v>
@@ -1158,7 +1151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="13.5" thickBot="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="20" t="s">
@@ -1194,15 +1187,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
@@ -1210,7 +1203,7 @@
     <col min="4" max="7" width="10.7109375" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="11" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1227,7 +1220,7 @@
         <v>54</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>48</v>
@@ -1239,13 +1232,13 @@
         <v>39</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="9" t="s">
         <v>31</v>
       </c>
@@ -1274,7 +1267,7 @@
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
@@ -1303,7 +1296,7 @@
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" s="9" t="s">
         <v>34</v>
       </c>
@@ -1332,7 +1325,7 @@
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="9" t="s">
         <v>36</v>
       </c>
@@ -1355,7 +1348,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="17" t="s">
         <v>50</v>
       </c>
@@ -1378,13 +1371,13 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -1401,15 +1394,15 @@
       </c>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>44</v>
@@ -1424,15 +1417,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>102</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>103</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>44</v>
@@ -1447,7 +1440,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="35"/>
     </row>
   </sheetData>
@@ -1459,20 +1452,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1483,7 +1476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1494,7 +1487,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1505,7 +1498,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1516,7 +1509,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1527,7 +1520,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1535,7 +1528,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="11.25" customHeight="1">
       <c r="A7" s="19" t="s">
         <v>63</v>
       </c>
@@ -1546,26 +1539,26 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="19" t="s">
         <v>65</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="19" t="s">
         <v>69</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>70</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added power sensor in DLC_test.xlsx
</commit_message>
<xml_diff>
--- a/wetb/dlc/tests/test_files/DLC_test.xlsx
+++ b/wetb/dlc/tests/test_files/DLC_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="19815" windowHeight="6855" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="18150" windowHeight="6375" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DLC" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -338,6 +338,18 @@
   </si>
   <si>
     <t>dlc%s_iec61400-1ed3</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Aerodynamic power</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>kW</t>
   </si>
 </sst>
 </file>
@@ -1197,10 +1209,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1333,7 +1345,7 @@
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>36</v>
       </c>
@@ -1356,84 +1368,84 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="14" t="s">
+    <row r="6" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="I6" s="12"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="8"/>
+        <v>50</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>51</v>
+      </c>
       <c r="C7" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+        <v>52</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="8">
-        <v>3</v>
-      </c>
-      <c r="I7" s="8">
-        <v>1</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>49</v>
-      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>98</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H8" s="8">
+        <v>3</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>98</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>44</v>
@@ -1448,8 +1460,36 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="35"/>
+    <row r="10" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="35"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>